<commit_message>
update data, new path for digital ocean
</commit_message>
<xml_diff>
--- a/games/cozy-grove/cozy-grove_data.xlsx
+++ b/games/cozy-grove/cozy-grove_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubChelsea\Achievement-Vault\games\cozy-grove\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3129845-060D-499E-BE46-C72A1848D75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF7E6A1-92A7-4F8B-A953-7ADE719ED78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="1005" windowWidth="21600" windowHeight="13830" xr2:uid="{E79D6183-D772-F644-AE89-4CAD504C8F4D}"/>
+    <workbookView xWindow="3120" yWindow="1410" windowWidth="21600" windowHeight="13830" xr2:uid="{E79D6183-D772-F644-AE89-4CAD504C8F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6124,16 +6124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6474,219 +6470,220 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4659E671-0874-FE42-985B-794BDDF20B74}">
   <dimension ref="A1:BP255"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="J83" workbookViewId="0">
+      <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.5" style="3" customWidth="1"/>
-    <col min="3" max="4" width="6.5" style="3" customWidth="1"/>
+    <col min="1" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="4" width="6.5" customWidth="1"/>
+    <col min="17" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>1279</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="W1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="3" t="s">
         <v>1280</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="3" t="s">
         <v>1282</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" s="3" t="s">
         <v>1283</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AL1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AM1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AQ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AS1" s="3" t="s">
         <v>1285</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AU1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AX1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AY1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="3" t="s">
         <v>1288</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BC1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BC1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" s="3" t="s">
         <v>1287</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BF1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BG1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BG1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BI1" s="3" t="s">
         <v>1289</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BK1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BK1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BM1" s="3" t="s">
         <v>1290</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BN1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="BO1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BO1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BP1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6697,7 +6694,7 @@
       <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -6852,7 +6849,7 @@
       <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="E3" t="s">
@@ -7007,7 +7004,7 @@
       <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="E4" t="s">
@@ -7162,7 +7159,7 @@
       <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="E5" t="s">
@@ -7320,7 +7317,10 @@
       <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
@@ -7393,6 +7393,9 @@
         <v>1490</v>
       </c>
       <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
         <v>1</v>
       </c>
       <c r="AK6" t="s">
@@ -7478,7 +7481,7 @@
       <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="E7" t="s">
@@ -7639,7 +7642,7 @@
       <c r="B8" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="E8" t="s">
@@ -7800,7 +7803,7 @@
       <c r="B9" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="E9" t="s">
@@ -7961,7 +7964,7 @@
       <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -8125,7 +8128,7 @@
       <c r="B11" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -8174,6 +8177,9 @@
         <v>1316</v>
       </c>
       <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
         <v>1</v>
       </c>
       <c r="Y11" t="s">
@@ -8292,7 +8298,7 @@
       <c r="B12" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -8459,7 +8465,7 @@
       <c r="B13" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="E13" t="s">
@@ -8626,7 +8632,7 @@
       <c r="B14" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -8793,10 +8799,10 @@
       <c r="B15" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" t="s">
         <v>272</v>
       </c>
@@ -8843,6 +8849,9 @@
         <v>1320</v>
       </c>
       <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
         <v>1</v>
       </c>
       <c r="Y15" t="s">
@@ -8961,10 +8970,10 @@
       <c r="B16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" t="s">
         <v>273</v>
       </c>
@@ -9132,10 +9141,10 @@
       <c r="B17" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4"/>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" t="s">
         <v>274</v>
       </c>
@@ -9306,10 +9315,10 @@
       <c r="B18" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4"/>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" t="s">
         <v>275</v>
       </c>
@@ -9483,10 +9492,10 @@
       <c r="B19" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4"/>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" t="s">
         <v>276</v>
       </c>
@@ -9666,10 +9675,10 @@
       <c r="B20" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4"/>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" t="s">
         <v>277</v>
       </c>
@@ -9845,6 +9854,9 @@
         <v>1988</v>
       </c>
       <c r="BO20">
+        <v>1</v>
+      </c>
+      <c r="BP20">
         <v>1</v>
       </c>
     </row>
@@ -9855,10 +9867,10 @@
       <c r="B21" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4"/>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" t="s">
         <v>278</v>
       </c>
@@ -10050,10 +10062,10 @@
       <c r="B22" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" t="s">
         <v>279</v>
       </c>
@@ -10245,10 +10257,10 @@
       <c r="B23" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4"/>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" t="s">
         <v>280</v>
       </c>
@@ -10440,10 +10452,10 @@
       <c r="B24" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="E24" t="s">
         <v>281</v>
       </c>
@@ -10635,10 +10647,10 @@
       <c r="B25" t="s">
         <v>102</v>
       </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" t="s">
         <v>282</v>
       </c>
@@ -10833,10 +10845,10 @@
       <c r="B26" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4"/>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" t="s">
         <v>283</v>
       </c>
@@ -11031,7 +11043,7 @@
       <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="E27" t="s">
@@ -11228,7 +11240,7 @@
       <c r="B28" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="E28" t="s">
@@ -11425,7 +11437,7 @@
       <c r="B29" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="2">
         <v>1</v>
       </c>
       <c r="E29" t="s">
@@ -11622,7 +11634,7 @@
       <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="E30" t="s">
@@ -11819,7 +11831,7 @@
       <c r="B31" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="2">
         <v>1</v>
       </c>
       <c r="E31" t="s">
@@ -12016,7 +12028,7 @@
       <c r="B32" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <v>1</v>
       </c>
       <c r="E32" t="s">
@@ -12069,7 +12081,7 @@
       <c r="B33" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="E33" t="s">
@@ -12122,7 +12134,7 @@
       <c r="B34" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="2">
         <v>1</v>
       </c>
       <c r="E34" t="s">
@@ -12175,7 +12187,7 @@
       <c r="B35" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="2">
         <v>1</v>
       </c>
       <c r="E35" t="s">
@@ -12228,7 +12240,7 @@
       <c r="B36" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="2">
         <v>1</v>
       </c>
       <c r="E36" t="s">
@@ -12281,7 +12293,7 @@
       <c r="B37" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="2">
         <v>1</v>
       </c>
       <c r="E37" t="s">
@@ -12334,7 +12346,7 @@
       <c r="B38" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="E38" t="s">
@@ -12387,7 +12399,7 @@
       <c r="B39" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="2">
         <v>1</v>
       </c>
       <c r="E39" t="s">
@@ -12440,7 +12452,7 @@
       <c r="B40" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="2">
         <v>1</v>
       </c>
       <c r="E40" t="s">
@@ -12493,7 +12505,7 @@
       <c r="B41" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="E41" t="s">
@@ -12546,7 +12558,7 @@
       <c r="B42" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="2">
         <v>1</v>
       </c>
       <c r="E42" t="s">
@@ -12599,7 +12611,7 @@
       <c r="B43" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="E43" t="s">
@@ -12652,7 +12664,7 @@
       <c r="B44" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="2">
         <v>1</v>
       </c>
       <c r="E44" t="s">
@@ -12705,7 +12717,7 @@
       <c r="B45" t="s">
         <v>111</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="2">
         <v>1</v>
       </c>
       <c r="E45" t="s">
@@ -12758,7 +12770,7 @@
       <c r="B46" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="2">
         <v>1</v>
       </c>
       <c r="E46" t="s">
@@ -12811,7 +12823,7 @@
       <c r="B47" t="s">
         <v>92</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="2">
         <v>1</v>
       </c>
       <c r="E47" t="s">
@@ -12864,7 +12876,7 @@
       <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="2">
         <v>1</v>
       </c>
       <c r="E48" t="s">
@@ -12917,7 +12929,7 @@
       <c r="B49" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="2">
         <v>1</v>
       </c>
       <c r="E49" t="s">
@@ -12970,7 +12982,7 @@
       <c r="B50" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="2">
         <v>1</v>
       </c>
       <c r="E50" t="s">
@@ -13023,7 +13035,7 @@
       <c r="B51" t="s">
         <v>98</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="E51" t="s">
@@ -13076,7 +13088,7 @@
       <c r="B52" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="2">
         <v>1</v>
       </c>
       <c r="E52" t="s">
@@ -13129,7 +13141,7 @@
       <c r="B53" t="s">
         <v>89</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="2">
         <v>1</v>
       </c>
       <c r="E53" t="s">
@@ -13182,7 +13194,7 @@
       <c r="B54" t="s">
         <v>103</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="2">
         <v>1</v>
       </c>
       <c r="E54" t="s">
@@ -13235,7 +13247,7 @@
       <c r="B55" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="2">
         <v>1</v>
       </c>
       <c r="E55" t="s">
@@ -13288,7 +13300,7 @@
       <c r="B56" t="s">
         <v>101</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C56" s="2">
         <v>1</v>
       </c>
       <c r="E56" t="s">
@@ -13341,7 +13353,7 @@
       <c r="B57" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="2">
         <v>1</v>
       </c>
       <c r="E57" t="s">
@@ -13394,7 +13406,7 @@
       <c r="B58" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="4">
+      <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="E58" t="s">
@@ -13447,7 +13459,7 @@
       <c r="B59" t="s">
         <v>107</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="2">
         <v>1</v>
       </c>
       <c r="E59" t="s">
@@ -13500,7 +13512,7 @@
       <c r="B60" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="2">
         <v>1</v>
       </c>
       <c r="E60" t="s">
@@ -13553,7 +13565,7 @@
       <c r="B61" t="s">
         <v>98</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C61" s="2">
         <v>1</v>
       </c>
       <c r="E61" t="s">
@@ -13606,7 +13618,7 @@
       <c r="B62" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="4">
+      <c r="C62" s="2">
         <v>1</v>
       </c>
       <c r="E62" t="s">
@@ -13659,7 +13671,7 @@
       <c r="B63" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="4">
+      <c r="C63" s="2">
         <v>1</v>
       </c>
       <c r="E63" t="s">
@@ -13712,7 +13724,7 @@
       <c r="B64" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="4">
+      <c r="C64" s="2">
         <v>1</v>
       </c>
       <c r="E64" t="s">
@@ -13758,14 +13770,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C65" s="2">
         <v>1</v>
       </c>
       <c r="E65" t="s">
@@ -13811,14 +13823,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>107</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="2">
         <v>1</v>
       </c>
       <c r="E66" t="s">
@@ -13864,14 +13876,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>69</v>
       </c>
       <c r="B67" t="s">
         <v>117</v>
       </c>
-      <c r="C67" s="4">
+      <c r="C67" s="2">
         <v>1</v>
       </c>
       <c r="E67" t="s">
@@ -13917,14 +13929,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
       <c r="B68" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="4">
+      <c r="C68" s="2">
         <v>1</v>
       </c>
       <c r="E68" t="s">
@@ -13970,14 +13982,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>71</v>
       </c>
       <c r="B69" t="s">
         <v>109</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="2">
         <v>1</v>
       </c>
       <c r="E69" t="s">
@@ -14022,15 +14034,18 @@
       <c r="S69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="4">
+      <c r="C70" s="2">
         <v>1</v>
       </c>
       <c r="E70" t="s">
@@ -14064,14 +14079,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="2">
         <v>1</v>
       </c>
       <c r="E71" t="s">
@@ -14105,14 +14120,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>118</v>
       </c>
-      <c r="C72" s="4">
+      <c r="C72" s="2">
         <v>1</v>
       </c>
       <c r="E72" t="s">
@@ -14146,14 +14161,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>98</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="2">
         <v>1</v>
       </c>
       <c r="E73" t="s">
@@ -14187,14 +14202,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>117</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="2">
         <v>1</v>
       </c>
       <c r="E74" t="s">
@@ -14228,14 +14243,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>116</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="2">
         <v>1</v>
       </c>
       <c r="E75" t="s">
@@ -14269,14 +14284,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="2">
         <v>1</v>
       </c>
       <c r="E76" t="s">
@@ -14310,14 +14325,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>106</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="2">
         <v>1</v>
       </c>
       <c r="E77" t="s">
@@ -14351,14 +14366,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78" s="2">
         <v>1</v>
       </c>
       <c r="E78" t="s">
@@ -14392,14 +14407,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
       <c r="B79" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="2">
         <v>1</v>
       </c>
       <c r="E79" t="s">
@@ -14433,14 +14448,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
       <c r="B80" t="s">
         <v>112</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+      <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
@@ -14481,7 +14499,7 @@
       <c r="B81" t="s">
         <v>117</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="2">
         <v>1</v>
       </c>
       <c r="E81" t="s">
@@ -14522,7 +14540,7 @@
       <c r="B82" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="2">
         <v>1</v>
       </c>
       <c r="E82" t="s">
@@ -14563,7 +14581,7 @@
       <c r="B83" t="s">
         <v>98</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83" s="2">
         <v>1</v>
       </c>
       <c r="E83" t="s">
@@ -14604,7 +14622,7 @@
       <c r="B84" t="s">
         <v>109</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="2">
         <v>1</v>
       </c>
       <c r="E84" t="s">
@@ -14645,7 +14663,7 @@
       <c r="B85" t="s">
         <v>115</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="2">
         <v>1</v>
       </c>
       <c r="E85" t="s">
@@ -14686,10 +14704,10 @@
       <c r="B86" t="s">
         <v>119</v>
       </c>
-      <c r="C86" s="4">
-        <v>1</v>
-      </c>
-      <c r="D86" s="4">
+      <c r="C86" s="2">
+        <v>1</v>
+      </c>
+      <c r="D86" s="2">
         <v>1</v>
       </c>
       <c r="E86" t="s">
@@ -14730,10 +14748,10 @@
       <c r="B87" t="s">
         <v>120</v>
       </c>
-      <c r="C87" s="4">
-        <v>1</v>
-      </c>
-      <c r="D87" s="4">
+      <c r="C87" s="2">
+        <v>1</v>
+      </c>
+      <c r="D87" s="2">
         <v>1</v>
       </c>
       <c r="E87" t="s">
@@ -14774,10 +14792,10 @@
       <c r="B88" t="s">
         <v>121</v>
       </c>
-      <c r="C88" s="4">
-        <v>1</v>
-      </c>
-      <c r="D88" s="4">
+      <c r="C88" s="2">
+        <v>1</v>
+      </c>
+      <c r="D88" s="2">
         <v>1</v>
       </c>
       <c r="E88" t="s">
@@ -14818,10 +14836,10 @@
       <c r="B89" t="s">
         <v>105</v>
       </c>
-      <c r="C89" s="4">
-        <v>1</v>
-      </c>
-      <c r="D89" s="4">
+      <c r="C89" s="2">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2">
         <v>1</v>
       </c>
       <c r="E89" t="s">
@@ -14865,10 +14883,10 @@
       <c r="B90" t="s">
         <v>122</v>
       </c>
-      <c r="C90" s="4">
-        <v>1</v>
-      </c>
-      <c r="D90" s="4">
+      <c r="C90" s="2">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2">
         <v>1</v>
       </c>
       <c r="E90" t="s">
@@ -14912,10 +14930,10 @@
       <c r="B91" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="4">
-        <v>1</v>
-      </c>
-      <c r="D91" s="4">
+      <c r="C91" s="2">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2">
         <v>1</v>
       </c>
       <c r="E91" t="s">
@@ -14959,10 +14977,10 @@
       <c r="B92" t="s">
         <v>124</v>
       </c>
-      <c r="C92" s="4">
-        <v>1</v>
-      </c>
-      <c r="D92" s="4">
+      <c r="C92" s="2">
+        <v>1</v>
+      </c>
+      <c r="D92" s="2">
         <v>1</v>
       </c>
       <c r="E92" t="s">
@@ -15006,10 +15024,10 @@
       <c r="B93" t="s">
         <v>125</v>
       </c>
-      <c r="C93" s="4">
-        <v>1</v>
-      </c>
-      <c r="D93" s="4">
+      <c r="C93" s="2">
+        <v>1</v>
+      </c>
+      <c r="D93" s="2">
         <v>1</v>
       </c>
       <c r="E93" t="s">
@@ -15053,10 +15071,10 @@
       <c r="B94" t="s">
         <v>126</v>
       </c>
-      <c r="C94" s="4">
-        <v>1</v>
-      </c>
-      <c r="D94" s="4">
+      <c r="C94" s="2">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
         <v>1</v>
       </c>
       <c r="E94" t="s">
@@ -15100,10 +15118,10 @@
       <c r="B95" t="s">
         <v>122</v>
       </c>
-      <c r="C95" s="4">
-        <v>1</v>
-      </c>
-      <c r="D95" s="4">
+      <c r="C95" s="2">
+        <v>1</v>
+      </c>
+      <c r="D95" s="2">
         <v>1</v>
       </c>
       <c r="E95" t="s">
@@ -15147,10 +15165,10 @@
       <c r="B96" t="s">
         <v>120</v>
       </c>
-      <c r="C96" s="4">
-        <v>1</v>
-      </c>
-      <c r="D96" s="4">
+      <c r="C96" s="2">
+        <v>1</v>
+      </c>
+      <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96" t="s">
@@ -15187,17 +15205,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>160</v>
       </c>
       <c r="B97" t="s">
         <v>127</v>
       </c>
-      <c r="C97" s="4">
-        <v>1</v>
-      </c>
-      <c r="D97" s="4">
+      <c r="C97" s="2">
+        <v>1</v>
+      </c>
+      <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97" t="s">
@@ -15233,18 +15251,21 @@
       <c r="S97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>161</v>
       </c>
       <c r="B98" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="4">
-        <v>1</v>
-      </c>
-      <c r="D98" s="4">
+      <c r="C98" s="2">
+        <v>1</v>
+      </c>
+      <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" t="s">
@@ -15281,17 +15302,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>162</v>
       </c>
       <c r="B99" t="s">
         <v>129</v>
       </c>
-      <c r="C99" s="4">
-        <v>1</v>
-      </c>
-      <c r="D99" s="4">
+      <c r="C99" s="2">
+        <v>1</v>
+      </c>
+      <c r="D99" s="2">
         <v>1</v>
       </c>
       <c r="E99" t="s">
@@ -15328,17 +15349,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>163</v>
       </c>
       <c r="B100" t="s">
         <v>130</v>
       </c>
-      <c r="C100" s="4">
-        <v>1</v>
-      </c>
-      <c r="D100" s="4">
+      <c r="C100" s="2">
+        <v>1</v>
+      </c>
+      <c r="D100" s="2">
         <v>1</v>
       </c>
       <c r="E100" t="s">
@@ -15375,17 +15396,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>164</v>
       </c>
       <c r="B101" t="s">
         <v>120</v>
       </c>
-      <c r="C101" s="4">
-        <v>1</v>
-      </c>
-      <c r="D101" s="4">
+      <c r="C101" s="2">
+        <v>1</v>
+      </c>
+      <c r="D101" s="2">
         <v>1</v>
       </c>
       <c r="E101" t="s">
@@ -15422,17 +15443,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>165</v>
       </c>
       <c r="B102" t="s">
         <v>131</v>
       </c>
-      <c r="C102" s="4">
-        <v>1</v>
-      </c>
-      <c r="D102" s="4">
+      <c r="C102" s="2">
+        <v>1</v>
+      </c>
+      <c r="D102" s="2">
         <v>1</v>
       </c>
       <c r="E102" t="s">
@@ -15469,17 +15490,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>166</v>
       </c>
       <c r="B103" t="s">
         <v>132</v>
       </c>
-      <c r="C103" s="4">
-        <v>1</v>
-      </c>
-      <c r="D103" s="4">
+      <c r="C103" s="2">
+        <v>1</v>
+      </c>
+      <c r="D103" s="2">
         <v>1</v>
       </c>
       <c r="E103" t="s">
@@ -15516,17 +15537,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>167</v>
       </c>
       <c r="B104" t="s">
         <v>133</v>
       </c>
-      <c r="C104" s="4">
-        <v>1</v>
-      </c>
-      <c r="D104" s="4">
+      <c r="C104" s="2">
+        <v>1</v>
+      </c>
+      <c r="D104" s="2">
         <v>1</v>
       </c>
       <c r="E104" t="s">
@@ -15563,17 +15584,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>168</v>
       </c>
       <c r="B105" t="s">
         <v>124</v>
       </c>
-      <c r="C105" s="4">
-        <v>1</v>
-      </c>
-      <c r="D105" s="4">
+      <c r="C105" s="2">
+        <v>1</v>
+      </c>
+      <c r="D105" s="2">
         <v>1</v>
       </c>
       <c r="E105" t="s">
@@ -15610,17 +15631,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>169</v>
       </c>
       <c r="B106" t="s">
         <v>134</v>
       </c>
-      <c r="C106" s="4">
-        <v>1</v>
-      </c>
-      <c r="D106" s="4">
+      <c r="C106" s="2">
+        <v>1</v>
+      </c>
+      <c r="D106" s="2">
         <v>1</v>
       </c>
       <c r="E106" t="s">
@@ -15657,17 +15678,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>170</v>
       </c>
       <c r="B107" t="s">
         <v>135</v>
       </c>
-      <c r="C107" s="4">
-        <v>1</v>
-      </c>
-      <c r="D107" s="4">
+      <c r="C107" s="2">
+        <v>1</v>
+      </c>
+      <c r="D107" s="2">
         <v>1</v>
       </c>
       <c r="E107" t="s">
@@ -15704,17 +15725,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>171</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
       </c>
-      <c r="C108" s="4">
-        <v>1</v>
-      </c>
-      <c r="D108" s="4">
+      <c r="C108" s="2">
+        <v>1</v>
+      </c>
+      <c r="D108" s="2">
         <v>1</v>
       </c>
       <c r="E108" t="s">
@@ -15751,17 +15772,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>172</v>
       </c>
       <c r="B109" t="s">
         <v>137</v>
       </c>
-      <c r="C109" s="4">
-        <v>1</v>
-      </c>
-      <c r="D109" s="4">
+      <c r="C109" s="2">
+        <v>1</v>
+      </c>
+      <c r="D109" s="2">
         <v>1</v>
       </c>
       <c r="E109" t="s">
@@ -15798,17 +15819,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>173</v>
       </c>
       <c r="B110" t="s">
         <v>138</v>
       </c>
-      <c r="C110" s="4">
-        <v>1</v>
-      </c>
-      <c r="D110" s="4">
+      <c r="C110" s="2">
+        <v>1</v>
+      </c>
+      <c r="D110" s="2">
         <v>1</v>
       </c>
       <c r="E110" t="s">
@@ -15845,17 +15866,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>174</v>
       </c>
       <c r="B111" t="s">
         <v>128</v>
       </c>
-      <c r="C111" s="4">
-        <v>1</v>
-      </c>
-      <c r="D111" s="4">
+      <c r="C111" s="2">
+        <v>1</v>
+      </c>
+      <c r="D111" s="2">
         <v>1</v>
       </c>
       <c r="E111" t="s">
@@ -15892,17 +15913,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>175</v>
       </c>
       <c r="B112" t="s">
         <v>139</v>
       </c>
-      <c r="C112" s="4">
-        <v>1</v>
-      </c>
-      <c r="D112" s="4">
+      <c r="C112" s="2">
+        <v>1</v>
+      </c>
+      <c r="D112" s="2">
         <v>1</v>
       </c>
       <c r="E112" t="s">
@@ -15946,10 +15967,10 @@
       <c r="B113" t="s">
         <v>140</v>
       </c>
-      <c r="C113" s="4">
-        <v>1</v>
-      </c>
-      <c r="D113" s="4">
+      <c r="C113" s="2">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2">
         <v>1</v>
       </c>
       <c r="E113" t="s">
@@ -15993,10 +16014,10 @@
       <c r="B114" t="s">
         <v>96</v>
       </c>
-      <c r="C114" s="4">
-        <v>1</v>
-      </c>
-      <c r="D114" s="4">
+      <c r="C114" s="2">
+        <v>1</v>
+      </c>
+      <c r="D114" s="2">
         <v>1</v>
       </c>
       <c r="E114" t="s">
@@ -16040,10 +16061,10 @@
       <c r="B115" t="s">
         <v>141</v>
       </c>
-      <c r="C115" s="4">
-        <v>1</v>
-      </c>
-      <c r="D115" s="4">
+      <c r="C115" s="2">
+        <v>1</v>
+      </c>
+      <c r="D115" s="2">
         <v>1</v>
       </c>
       <c r="E115" t="s">
@@ -16087,10 +16108,10 @@
       <c r="B116" t="s">
         <v>119</v>
       </c>
-      <c r="C116" s="4">
-        <v>1</v>
-      </c>
-      <c r="D116" s="4">
+      <c r="C116" s="2">
+        <v>1</v>
+      </c>
+      <c r="D116" s="2">
         <v>1</v>
       </c>
       <c r="E116" t="s">
@@ -16134,10 +16155,10 @@
       <c r="B117" t="s">
         <v>142</v>
       </c>
-      <c r="C117" s="4">
-        <v>1</v>
-      </c>
-      <c r="D117" s="4">
+      <c r="C117" s="2">
+        <v>1</v>
+      </c>
+      <c r="D117" s="2">
         <v>1</v>
       </c>
       <c r="E117" t="s">
@@ -16181,10 +16202,10 @@
       <c r="B118" t="s">
         <v>113</v>
       </c>
-      <c r="C118" s="4">
-        <v>1</v>
-      </c>
-      <c r="D118" s="4">
+      <c r="C118" s="2">
+        <v>1</v>
+      </c>
+      <c r="D118" s="2">
         <v>1</v>
       </c>
       <c r="E118" t="s">
@@ -16228,10 +16249,10 @@
       <c r="B119" t="s">
         <v>143</v>
       </c>
-      <c r="C119" s="4">
-        <v>1</v>
-      </c>
-      <c r="D119" s="4">
+      <c r="C119" s="2">
+        <v>1</v>
+      </c>
+      <c r="D119" s="2">
         <v>1</v>
       </c>
       <c r="E119" t="s">
@@ -16275,10 +16296,10 @@
       <c r="B120" t="s">
         <v>144</v>
       </c>
-      <c r="C120" s="4">
-        <v>1</v>
-      </c>
-      <c r="D120" s="4">
+      <c r="C120" s="2">
+        <v>1</v>
+      </c>
+      <c r="D120" s="2">
         <v>1</v>
       </c>
       <c r="E120" t="s">
@@ -16322,10 +16343,10 @@
       <c r="B121" t="s">
         <v>127</v>
       </c>
-      <c r="C121" s="4">
-        <v>1</v>
-      </c>
-      <c r="D121" s="4">
+      <c r="C121" s="2">
+        <v>1</v>
+      </c>
+      <c r="D121" s="2">
         <v>1</v>
       </c>
       <c r="E121" t="s">
@@ -16369,10 +16390,10 @@
       <c r="B122" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="4">
-        <v>1</v>
-      </c>
-      <c r="D122" s="4">
+      <c r="C122" s="2">
+        <v>1</v>
+      </c>
+      <c r="D122" s="2">
         <v>1</v>
       </c>
       <c r="E122" t="s">
@@ -16416,10 +16437,10 @@
       <c r="B123" t="s">
         <v>146</v>
       </c>
-      <c r="C123" s="4">
-        <v>1</v>
-      </c>
-      <c r="D123" s="4">
+      <c r="C123" s="2">
+        <v>1</v>
+      </c>
+      <c r="D123" s="2">
         <v>1</v>
       </c>
       <c r="E123" t="s">
@@ -16463,10 +16484,10 @@
       <c r="B124" t="s">
         <v>143</v>
       </c>
-      <c r="C124" s="4">
-        <v>1</v>
-      </c>
-      <c r="D124" s="4">
+      <c r="C124" s="2">
+        <v>1</v>
+      </c>
+      <c r="D124" s="2">
         <v>1</v>
       </c>
       <c r="E124" t="s">
@@ -16510,10 +16531,10 @@
       <c r="B125" t="s">
         <v>119</v>
       </c>
-      <c r="C125" s="4">
-        <v>1</v>
-      </c>
-      <c r="D125" s="4">
+      <c r="C125" s="2">
+        <v>1</v>
+      </c>
+      <c r="D125" s="2">
         <v>1</v>
       </c>
       <c r="E125" t="s">
@@ -16557,10 +16578,10 @@
       <c r="B126" t="s">
         <v>143</v>
       </c>
-      <c r="C126" s="4">
-        <v>1</v>
-      </c>
-      <c r="D126" s="4">
+      <c r="C126" s="2">
+        <v>1</v>
+      </c>
+      <c r="D126" s="2">
         <v>1</v>
       </c>
       <c r="E126" t="s">
@@ -16592,10 +16613,10 @@
       <c r="B127" t="s">
         <v>135</v>
       </c>
-      <c r="C127" s="4">
-        <v>1</v>
-      </c>
-      <c r="D127" s="4">
+      <c r="C127" s="2">
+        <v>1</v>
+      </c>
+      <c r="D127" s="2">
         <v>1</v>
       </c>
       <c r="E127" t="s">
@@ -16627,10 +16648,10 @@
       <c r="B128" t="s">
         <v>125</v>
       </c>
-      <c r="C128" s="4">
-        <v>1</v>
-      </c>
-      <c r="D128" s="4">
+      <c r="C128" s="2">
+        <v>1</v>
+      </c>
+      <c r="D128" s="2">
         <v>1</v>
       </c>
       <c r="E128" t="s">
@@ -16662,10 +16683,10 @@
       <c r="B129" t="s">
         <v>138</v>
       </c>
-      <c r="C129" s="4">
-        <v>1</v>
-      </c>
-      <c r="D129" s="4">
+      <c r="C129" s="2">
+        <v>1</v>
+      </c>
+      <c r="D129" s="2">
         <v>1</v>
       </c>
       <c r="E129" t="s">
@@ -16697,10 +16718,10 @@
       <c r="B130" t="s">
         <v>114</v>
       </c>
-      <c r="C130" s="4">
-        <v>1</v>
-      </c>
-      <c r="D130" s="4">
+      <c r="C130" s="2">
+        <v>1</v>
+      </c>
+      <c r="D130" s="2">
         <v>1</v>
       </c>
       <c r="E130" t="s">
@@ -16732,10 +16753,10 @@
       <c r="B131" t="s">
         <v>140</v>
       </c>
-      <c r="C131" s="4">
-        <v>1</v>
-      </c>
-      <c r="D131" s="4">
+      <c r="C131" s="2">
+        <v>1</v>
+      </c>
+      <c r="D131" s="2">
         <v>1</v>
       </c>
       <c r="E131" t="s">
@@ -16767,10 +16788,10 @@
       <c r="B132" t="s">
         <v>111</v>
       </c>
-      <c r="C132" s="4">
-        <v>1</v>
-      </c>
-      <c r="D132" s="4">
+      <c r="C132" s="2">
+        <v>1</v>
+      </c>
+      <c r="D132" s="2">
         <v>1</v>
       </c>
       <c r="E132" t="s">
@@ -16802,10 +16823,10 @@
       <c r="B133" t="s">
         <v>147</v>
       </c>
-      <c r="C133" s="4">
-        <v>1</v>
-      </c>
-      <c r="D133" s="4">
+      <c r="C133" s="2">
+        <v>1</v>
+      </c>
+      <c r="D133" s="2">
         <v>1</v>
       </c>
       <c r="E133" t="s">
@@ -16837,10 +16858,10 @@
       <c r="B134" t="s">
         <v>122</v>
       </c>
-      <c r="C134" s="4">
-        <v>1</v>
-      </c>
-      <c r="D134" s="4">
+      <c r="C134" s="2">
+        <v>1</v>
+      </c>
+      <c r="D134" s="2">
         <v>1</v>
       </c>
       <c r="E134" t="s">
@@ -16872,10 +16893,10 @@
       <c r="B135" t="s">
         <v>126</v>
       </c>
-      <c r="C135" s="4">
-        <v>1</v>
-      </c>
-      <c r="D135" s="4">
+      <c r="C135" s="2">
+        <v>1</v>
+      </c>
+      <c r="D135" s="2">
         <v>1</v>
       </c>
       <c r="E135" t="s">
@@ -16907,10 +16928,10 @@
       <c r="B136" t="s">
         <v>127</v>
       </c>
-      <c r="C136" s="4">
-        <v>1</v>
-      </c>
-      <c r="D136" s="4">
+      <c r="C136" s="2">
+        <v>1</v>
+      </c>
+      <c r="D136" s="2">
         <v>1</v>
       </c>
       <c r="E136" t="s">
@@ -16942,10 +16963,10 @@
       <c r="B137" t="s">
         <v>136</v>
       </c>
-      <c r="C137" s="4">
-        <v>1</v>
-      </c>
-      <c r="D137" s="4">
+      <c r="C137" s="2">
+        <v>1</v>
+      </c>
+      <c r="D137" s="2">
         <v>1</v>
       </c>
       <c r="E137" t="s">
@@ -16977,10 +16998,10 @@
       <c r="B138" t="s">
         <v>140</v>
       </c>
-      <c r="C138" s="4">
-        <v>1</v>
-      </c>
-      <c r="D138" s="4">
+      <c r="C138" s="2">
+        <v>1</v>
+      </c>
+      <c r="D138" s="2">
         <v>1</v>
       </c>
       <c r="E138" t="s">
@@ -17012,10 +17033,10 @@
       <c r="B139" t="s">
         <v>135</v>
       </c>
-      <c r="C139" s="4">
-        <v>1</v>
-      </c>
-      <c r="D139" s="4">
+      <c r="C139" s="2">
+        <v>1</v>
+      </c>
+      <c r="D139" s="2">
         <v>1</v>
       </c>
       <c r="E139" t="s">
@@ -17047,10 +17068,10 @@
       <c r="B140" t="s">
         <v>141</v>
       </c>
-      <c r="C140" s="4">
-        <v>1</v>
-      </c>
-      <c r="D140" s="4">
+      <c r="C140" s="2">
+        <v>1</v>
+      </c>
+      <c r="D140" s="2">
         <v>1</v>
       </c>
       <c r="E140" t="s">
@@ -17082,10 +17103,10 @@
       <c r="B141" t="s">
         <v>123</v>
       </c>
-      <c r="C141" s="4">
-        <v>1</v>
-      </c>
-      <c r="D141" s="4">
+      <c r="C141" s="2">
+        <v>1</v>
+      </c>
+      <c r="D141" s="2">
         <v>1</v>
       </c>
       <c r="E141" t="s">
@@ -17117,10 +17138,10 @@
       <c r="B142" t="s">
         <v>137</v>
       </c>
-      <c r="C142" s="4">
-        <v>1</v>
-      </c>
-      <c r="D142" s="4">
+      <c r="C142" s="2">
+        <v>1</v>
+      </c>
+      <c r="D142" s="2">
         <v>1</v>
       </c>
       <c r="E142" t="s">
@@ -17152,10 +17173,10 @@
       <c r="B143" t="s">
         <v>144</v>
       </c>
-      <c r="C143" s="4">
-        <v>1</v>
-      </c>
-      <c r="D143" s="4">
+      <c r="C143" s="2">
+        <v>1</v>
+      </c>
+      <c r="D143" s="2">
         <v>1</v>
       </c>
       <c r="E143" t="s">
@@ -17187,10 +17208,10 @@
       <c r="B144" t="s">
         <v>146</v>
       </c>
-      <c r="C144" s="4">
-        <v>1</v>
-      </c>
-      <c r="D144" s="4">
+      <c r="C144" s="2">
+        <v>1</v>
+      </c>
+      <c r="D144" s="2">
         <v>1</v>
       </c>
       <c r="E144" t="s">
@@ -17215,17 +17236,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>208</v>
       </c>
       <c r="B145" t="s">
         <v>130</v>
       </c>
-      <c r="C145" s="4">
-        <v>1</v>
-      </c>
-      <c r="D145" s="4">
+      <c r="C145" s="2">
+        <v>1</v>
+      </c>
+      <c r="D145" s="2">
         <v>1</v>
       </c>
       <c r="E145" t="s">
@@ -17250,17 +17271,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>209</v>
       </c>
       <c r="B146" t="s">
         <v>118</v>
       </c>
-      <c r="C146" s="4">
-        <v>1</v>
-      </c>
-      <c r="D146" s="4">
+      <c r="C146" s="2">
+        <v>1</v>
+      </c>
+      <c r="D146" s="2">
         <v>1</v>
       </c>
       <c r="E146" t="s">
@@ -17285,17 +17306,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>210</v>
       </c>
       <c r="B147" t="s">
         <v>136</v>
       </c>
-      <c r="C147" s="4">
-        <v>1</v>
-      </c>
-      <c r="D147" s="4">
+      <c r="C147" s="2">
+        <v>1</v>
+      </c>
+      <c r="D147" s="2">
         <v>1</v>
       </c>
       <c r="E147" t="s">
@@ -17320,17 +17341,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>211</v>
       </c>
       <c r="B148" t="s">
         <v>144</v>
       </c>
-      <c r="C148" s="4">
-        <v>1</v>
-      </c>
-      <c r="D148" s="4">
+      <c r="C148" s="2">
+        <v>1</v>
+      </c>
+      <c r="D148" s="2">
         <v>1</v>
       </c>
       <c r="E148" t="s">
@@ -17355,17 +17376,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>212</v>
       </c>
       <c r="B149" t="s">
         <v>128</v>
       </c>
-      <c r="C149" s="4">
-        <v>1</v>
-      </c>
-      <c r="D149" s="4">
+      <c r="C149" s="2">
+        <v>1</v>
+      </c>
+      <c r="D149" s="2">
         <v>1</v>
       </c>
       <c r="E149" t="s">
@@ -17389,18 +17410,21 @@
       <c r="S149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>213</v>
       </c>
       <c r="B150" t="s">
         <v>100</v>
       </c>
-      <c r="C150" s="4">
-        <v>1</v>
-      </c>
-      <c r="D150" s="4">
+      <c r="C150" s="2">
+        <v>1</v>
+      </c>
+      <c r="D150" s="2">
         <v>1</v>
       </c>
       <c r="E150" t="s">
@@ -17425,17 +17449,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>214</v>
       </c>
       <c r="B151" t="s">
         <v>148</v>
       </c>
-      <c r="C151" s="4">
-        <v>1</v>
-      </c>
-      <c r="D151" s="4">
+      <c r="C151" s="2">
+        <v>1</v>
+      </c>
+      <c r="D151" s="2">
         <v>1</v>
       </c>
       <c r="E151" t="s">
@@ -17460,17 +17484,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>215</v>
       </c>
       <c r="B152" t="s">
         <v>132</v>
       </c>
-      <c r="C152" s="4">
-        <v>1</v>
-      </c>
-      <c r="D152" s="4">
+      <c r="C152" s="2">
+        <v>1</v>
+      </c>
+      <c r="D152" s="2">
         <v>1</v>
       </c>
       <c r="E152" t="s">
@@ -17495,17 +17519,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>216</v>
       </c>
       <c r="B153" t="s">
         <v>141</v>
       </c>
-      <c r="C153" s="4">
-        <v>1</v>
-      </c>
-      <c r="D153" s="4">
+      <c r="C153" s="2">
+        <v>1</v>
+      </c>
+      <c r="D153" s="2">
         <v>1</v>
       </c>
       <c r="E153" t="s">
@@ -17530,17 +17554,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>217</v>
       </c>
       <c r="B154" t="s">
         <v>134</v>
       </c>
-      <c r="C154" s="4">
-        <v>1</v>
-      </c>
-      <c r="D154" s="4">
+      <c r="C154" s="2">
+        <v>1</v>
+      </c>
+      <c r="D154" s="2">
         <v>1</v>
       </c>
       <c r="E154" t="s">
@@ -17565,17 +17589,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>218</v>
       </c>
       <c r="B155" t="s">
         <v>114</v>
       </c>
-      <c r="C155" s="4">
-        <v>1</v>
-      </c>
-      <c r="D155" s="4">
+      <c r="C155" s="2">
+        <v>1</v>
+      </c>
+      <c r="D155" s="2">
         <v>1</v>
       </c>
       <c r="E155" t="s">
@@ -17599,18 +17623,21 @@
       <c r="S155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>219</v>
       </c>
       <c r="B156" t="s">
         <v>129</v>
       </c>
-      <c r="C156" s="4">
-        <v>1</v>
-      </c>
-      <c r="D156" s="4">
+      <c r="C156" s="2">
+        <v>1</v>
+      </c>
+      <c r="D156" s="2">
         <v>1</v>
       </c>
       <c r="E156" t="s">
@@ -17635,17 +17662,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>220</v>
       </c>
       <c r="B157" t="s">
         <v>137</v>
       </c>
-      <c r="C157" s="4">
-        <v>1</v>
-      </c>
-      <c r="D157" s="4">
+      <c r="C157" s="2">
+        <v>1</v>
+      </c>
+      <c r="D157" s="2">
         <v>1</v>
       </c>
       <c r="E157" t="s">
@@ -17670,17 +17697,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>221</v>
       </c>
       <c r="B158" t="s">
         <v>120</v>
       </c>
-      <c r="C158" s="4">
-        <v>1</v>
-      </c>
-      <c r="D158" s="4">
+      <c r="C158" s="2">
+        <v>1</v>
+      </c>
+      <c r="D158" s="2">
         <v>1</v>
       </c>
       <c r="E158" t="s">
@@ -17705,17 +17732,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>222</v>
       </c>
       <c r="B159" t="s">
         <v>125</v>
       </c>
-      <c r="C159" s="4">
-        <v>1</v>
-      </c>
-      <c r="D159" s="4">
+      <c r="C159" s="2">
+        <v>1</v>
+      </c>
+      <c r="D159" s="2">
         <v>1</v>
       </c>
       <c r="E159" t="s">
@@ -17740,17 +17767,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>223</v>
       </c>
       <c r="B160" t="s">
         <v>130</v>
       </c>
-      <c r="C160" s="4">
-        <v>1</v>
-      </c>
-      <c r="D160" s="4">
+      <c r="C160" s="2">
+        <v>1</v>
+      </c>
+      <c r="D160" s="2">
         <v>1</v>
       </c>
       <c r="E160" t="s">
@@ -17782,10 +17809,10 @@
       <c r="B161" t="s">
         <v>142</v>
       </c>
-      <c r="C161" s="4">
-        <v>1</v>
-      </c>
-      <c r="D161" s="4">
+      <c r="C161" s="2">
+        <v>1</v>
+      </c>
+      <c r="D161" s="2">
         <v>1</v>
       </c>
       <c r="E161" t="s">
@@ -17817,10 +17844,10 @@
       <c r="B162" t="s">
         <v>124</v>
       </c>
-      <c r="C162" s="4">
-        <v>1</v>
-      </c>
-      <c r="D162" s="4">
+      <c r="C162" s="2">
+        <v>1</v>
+      </c>
+      <c r="D162" s="2">
         <v>1</v>
       </c>
       <c r="E162" t="s">
@@ -17852,10 +17879,10 @@
       <c r="B163" t="s">
         <v>120</v>
       </c>
-      <c r="C163" s="4">
-        <v>1</v>
-      </c>
-      <c r="D163" s="4">
+      <c r="C163" s="2">
+        <v>1</v>
+      </c>
+      <c r="D163" s="2">
         <v>1</v>
       </c>
       <c r="E163" t="s">
@@ -17887,10 +17914,10 @@
       <c r="B164" t="s">
         <v>111</v>
       </c>
-      <c r="C164" s="4">
-        <v>1</v>
-      </c>
-      <c r="D164" s="4">
+      <c r="C164" s="2">
+        <v>1</v>
+      </c>
+      <c r="D164" s="2">
         <v>1</v>
       </c>
       <c r="E164" t="s">
@@ -17922,10 +17949,10 @@
       <c r="B165" t="s">
         <v>126</v>
       </c>
-      <c r="C165" s="4">
-        <v>1</v>
-      </c>
-      <c r="D165" s="4">
+      <c r="C165" s="2">
+        <v>1</v>
+      </c>
+      <c r="D165" s="2">
         <v>1</v>
       </c>
       <c r="E165" t="s">
@@ -17957,10 +17984,10 @@
       <c r="B166" t="s">
         <v>129</v>
       </c>
-      <c r="C166" s="4">
-        <v>1</v>
-      </c>
-      <c r="D166" s="4">
+      <c r="C166" s="2">
+        <v>1</v>
+      </c>
+      <c r="D166" s="2">
         <v>1</v>
       </c>
       <c r="E166" t="s">
@@ -17992,10 +18019,10 @@
       <c r="B167" t="s">
         <v>142</v>
       </c>
-      <c r="C167" s="4">
-        <v>1</v>
-      </c>
-      <c r="D167" s="4">
+      <c r="C167" s="2">
+        <v>1</v>
+      </c>
+      <c r="D167" s="2">
         <v>1</v>
       </c>
       <c r="E167" t="s">
@@ -18027,10 +18054,10 @@
       <c r="B168" t="s">
         <v>139</v>
       </c>
-      <c r="C168" s="4">
-        <v>1</v>
-      </c>
-      <c r="D168" s="4">
+      <c r="C168" s="2">
+        <v>1</v>
+      </c>
+      <c r="D168" s="2">
         <v>1</v>
       </c>
       <c r="E168" t="s">
@@ -18062,10 +18089,10 @@
       <c r="B169" t="s">
         <v>100</v>
       </c>
-      <c r="C169" s="4">
-        <v>1</v>
-      </c>
-      <c r="D169" s="4">
+      <c r="C169" s="2">
+        <v>1</v>
+      </c>
+      <c r="D169" s="2">
         <v>1</v>
       </c>
       <c r="E169" t="s">
@@ -18097,10 +18124,10 @@
       <c r="B170" t="s">
         <v>123</v>
       </c>
-      <c r="C170" s="4">
-        <v>1</v>
-      </c>
-      <c r="D170" s="4">
+      <c r="C170" s="2">
+        <v>1</v>
+      </c>
+      <c r="D170" s="2">
         <v>1</v>
       </c>
       <c r="E170" t="s">
@@ -18132,10 +18159,10 @@
       <c r="B171" t="s">
         <v>147</v>
       </c>
-      <c r="C171" s="4">
-        <v>1</v>
-      </c>
-      <c r="D171" s="4">
+      <c r="C171" s="2">
+        <v>1</v>
+      </c>
+      <c r="D171" s="2">
         <v>1</v>
       </c>
       <c r="E171" t="s">
@@ -18167,10 +18194,10 @@
       <c r="B172" t="s">
         <v>113</v>
       </c>
-      <c r="C172" s="4">
-        <v>1</v>
-      </c>
-      <c r="D172" s="4">
+      <c r="C172" s="2">
+        <v>1</v>
+      </c>
+      <c r="D172" s="2">
         <v>1</v>
       </c>
       <c r="E172" t="s">
@@ -18202,10 +18229,10 @@
       <c r="B173" t="s">
         <v>134</v>
       </c>
-      <c r="C173" s="4">
-        <v>1</v>
-      </c>
-      <c r="D173" s="4">
+      <c r="C173" s="2">
+        <v>1</v>
+      </c>
+      <c r="D173" s="2">
         <v>1</v>
       </c>
       <c r="E173" t="s">
@@ -18240,10 +18267,10 @@
       <c r="B174" t="s">
         <v>118</v>
       </c>
-      <c r="C174" s="4">
-        <v>1</v>
-      </c>
-      <c r="D174" s="4">
+      <c r="C174" s="2">
+        <v>1</v>
+      </c>
+      <c r="D174" s="2">
         <v>1</v>
       </c>
       <c r="E174" t="s">
@@ -18278,10 +18305,10 @@
       <c r="B175" t="s">
         <v>133</v>
       </c>
-      <c r="C175" s="4">
-        <v>1</v>
-      </c>
-      <c r="D175" s="4">
+      <c r="C175" s="2">
+        <v>1</v>
+      </c>
+      <c r="D175" s="2">
         <v>1</v>
       </c>
       <c r="E175" t="s">
@@ -18316,10 +18343,10 @@
       <c r="B176" t="s">
         <v>90</v>
       </c>
-      <c r="C176" s="4">
-        <v>1</v>
-      </c>
-      <c r="D176" s="4">
+      <c r="C176" s="2">
+        <v>1</v>
+      </c>
+      <c r="D176" s="2">
         <v>1</v>
       </c>
       <c r="E176" t="s">
@@ -18354,10 +18381,10 @@
       <c r="B177" t="s">
         <v>145</v>
       </c>
-      <c r="C177" s="4">
-        <v>1</v>
-      </c>
-      <c r="D177" s="4">
+      <c r="C177" s="2">
+        <v>1</v>
+      </c>
+      <c r="D177" s="2">
         <v>1</v>
       </c>
       <c r="E177" t="s">
@@ -18392,10 +18419,10 @@
       <c r="B178" t="s">
         <v>133</v>
       </c>
-      <c r="C178" s="4">
-        <v>1</v>
-      </c>
-      <c r="D178" s="4">
+      <c r="C178" s="2">
+        <v>1</v>
+      </c>
+      <c r="D178" s="2">
         <v>1</v>
       </c>
       <c r="E178" t="s">
@@ -18430,10 +18457,10 @@
       <c r="B179" t="s">
         <v>147</v>
       </c>
-      <c r="C179" s="4">
-        <v>1</v>
-      </c>
-      <c r="D179" s="4">
+      <c r="C179" s="2">
+        <v>1</v>
+      </c>
+      <c r="D179" s="2">
         <v>1</v>
       </c>
       <c r="E179" t="s">
@@ -18468,10 +18495,10 @@
       <c r="B180" t="s">
         <v>145</v>
       </c>
-      <c r="C180" s="4">
-        <v>1</v>
-      </c>
-      <c r="D180" s="4">
+      <c r="C180" s="2">
+        <v>1</v>
+      </c>
+      <c r="D180" s="2">
         <v>1</v>
       </c>
       <c r="E180" t="s">
@@ -18506,10 +18533,10 @@
       <c r="B181" t="s">
         <v>138</v>
       </c>
-      <c r="C181" s="4">
-        <v>1</v>
-      </c>
-      <c r="D181" s="4">
+      <c r="C181" s="2">
+        <v>1</v>
+      </c>
+      <c r="D181" s="2">
         <v>1</v>
       </c>
       <c r="E181" t="s">
@@ -18544,10 +18571,10 @@
       <c r="B182" t="s">
         <v>131</v>
       </c>
-      <c r="C182" s="4">
-        <v>1</v>
-      </c>
-      <c r="D182" s="4">
+      <c r="C182" s="2">
+        <v>1</v>
+      </c>
+      <c r="D182" s="2">
         <v>1</v>
       </c>
       <c r="Q182" t="s">
@@ -18570,10 +18597,10 @@
       <c r="B183" t="s">
         <v>134</v>
       </c>
-      <c r="C183" s="4">
-        <v>1</v>
-      </c>
-      <c r="D183" s="4">
+      <c r="C183" s="2">
+        <v>1</v>
+      </c>
+      <c r="D183" s="2">
         <v>1</v>
       </c>
       <c r="Q183" t="s">
@@ -18596,10 +18623,10 @@
       <c r="B184" t="s">
         <v>139</v>
       </c>
-      <c r="C184" s="4">
-        <v>1</v>
-      </c>
-      <c r="D184" s="4">
+      <c r="C184" s="2">
+        <v>1</v>
+      </c>
+      <c r="D184" s="2">
         <v>1</v>
       </c>
       <c r="Q184" t="s">
@@ -18622,10 +18649,10 @@
       <c r="B185" t="s">
         <v>132</v>
       </c>
-      <c r="C185" s="4">
-        <v>1</v>
-      </c>
-      <c r="D185" s="4">
+      <c r="C185" s="2">
+        <v>1</v>
+      </c>
+      <c r="D185" s="2">
         <v>1</v>
       </c>
       <c r="Q185" t="s">
@@ -18648,10 +18675,10 @@
       <c r="B186" t="s">
         <v>148</v>
       </c>
-      <c r="C186" s="4">
-        <v>1</v>
-      </c>
-      <c r="D186" s="4">
+      <c r="C186" s="2">
+        <v>1</v>
+      </c>
+      <c r="D186" s="2">
         <v>1</v>
       </c>
       <c r="Q186" t="s">
@@ -18674,10 +18701,10 @@
       <c r="B187" t="s">
         <v>131</v>
       </c>
-      <c r="C187" s="4">
-        <v>1</v>
-      </c>
-      <c r="D187" s="4">
+      <c r="C187" s="2">
+        <v>1</v>
+      </c>
+      <c r="D187" s="2">
         <v>1</v>
       </c>
       <c r="Q187" t="s">
@@ -18700,10 +18727,10 @@
       <c r="B188" t="s">
         <v>121</v>
       </c>
-      <c r="C188" s="4">
-        <v>1</v>
-      </c>
-      <c r="D188" s="4">
+      <c r="C188" s="2">
+        <v>1</v>
+      </c>
+      <c r="D188" s="2">
         <v>1</v>
       </c>
       <c r="Q188" t="s">
@@ -18726,10 +18753,10 @@
       <c r="B189" t="s">
         <v>146</v>
       </c>
-      <c r="C189" s="4">
-        <v>1</v>
-      </c>
-      <c r="D189" s="4">
+      <c r="C189" s="2">
+        <v>1</v>
+      </c>
+      <c r="D189" s="2">
         <v>1</v>
       </c>
       <c r="Q189" t="s">
@@ -18746,10 +18773,10 @@
       <c r="B190" t="s">
         <v>121</v>
       </c>
-      <c r="C190" s="4">
-        <v>1</v>
-      </c>
-      <c r="D190" s="4">
+      <c r="C190" s="2">
+        <v>1</v>
+      </c>
+      <c r="D190" s="2">
         <v>1</v>
       </c>
       <c r="Q190" t="s">
@@ -18766,10 +18793,10 @@
       <c r="B191" t="s">
         <v>96</v>
       </c>
-      <c r="C191" s="4">
-        <v>1</v>
-      </c>
-      <c r="D191" s="4">
+      <c r="C191" s="2">
+        <v>1</v>
+      </c>
+      <c r="D191" s="2">
         <v>1</v>
       </c>
       <c r="Q191" t="s">
@@ -18786,10 +18813,10 @@
       <c r="B192" t="s">
         <v>134</v>
       </c>
-      <c r="C192" s="4">
-        <v>1</v>
-      </c>
-      <c r="D192" s="4">
+      <c r="C192" s="2">
+        <v>1</v>
+      </c>
+      <c r="D192" s="2">
         <v>1</v>
       </c>
       <c r="Q192" t="s">
@@ -18806,10 +18833,10 @@
       <c r="B193" t="s">
         <v>105</v>
       </c>
-      <c r="C193" s="4">
-        <v>1</v>
-      </c>
-      <c r="D193" s="4">
+      <c r="C193" s="2">
+        <v>1</v>
+      </c>
+      <c r="D193" s="2">
         <v>1</v>
       </c>
       <c r="Q193" t="s">
@@ -18826,10 +18853,10 @@
       <c r="B194" t="s">
         <v>148</v>
       </c>
-      <c r="C194" s="4">
-        <v>1</v>
-      </c>
-      <c r="D194" s="4">
+      <c r="C194" s="2">
+        <v>1</v>
+      </c>
+      <c r="D194" s="2">
         <v>1</v>
       </c>
       <c r="Q194" t="s">

</xml_diff>